<commit_message>
Global inline random number generator. Hw12
</commit_message>
<xml_diff>
--- a/xllfms/antithetic.xlsx
+++ b/xllfms/antithetic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\MATHGR5260_001_2018\xllfms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A8BCB7-A3B7-4328-9BCB-568563F49859}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E04A0CE-1855-43B9-8DBD-6BFF6DC90D64}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9983" xr2:uid="{6D9BEE77-D9DE-41D8-9399-1B471E16162A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="sigma">Sheet1!$C$10</definedName>
     <definedName name="t">Sheet1!$C$12</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,6 +73,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{801982AE-1787-40A3-A4AC-C680BAD6F497}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Use the cell above to generate lognormal variates with expeced value f and Var log F = sigma^2 t</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C16" authorId="0" shapeId="0" xr:uid="{5773BC2C-CFD4-48BB-A7B4-4E1A52628BC4}">
       <text>
         <r>
@@ -87,7 +101,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{BA18096D-81CE-450D-B9B4-50EF885991C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Put payoff with strike k.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C17" authorId="0" shapeId="0" xr:uid="{06F329CE-498A-4084-8C37-E98990F928E4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Use xllmonte to find the expected payoff.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{BE141F27-419B-43B8-B753-91C398A55B0A}">
       <text>
         <r>
           <rPr>
@@ -554,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE878AB-2193-436F-9A50-84199FEA8C5A}">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -579,19 +621,19 @@
       </c>
       <c r="C3">
         <f ca="1">RAND()</f>
-        <v>0.48628276649168822</v>
+        <v>0.77319011027449069</v>
       </c>
       <c r="D3">
         <f ca="1">C3^2</f>
-        <v>0.23647092898680977</v>
-      </c>
-      <c r="E3" t="e">
+        <v>0.59782294662627911</v>
+      </c>
+      <c r="E3">
         <f t="array" aca="1" ref="E3:F3" ca="1">_xll.MONTE.STDEV(D3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F3" t="e">
+        <v>0.33353481272362484</v>
+      </c>
+      <c r="F3">
         <f ca="1"/>
-        <v>#NAME?</v>
+        <v>0.29897151744356237</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.45">
@@ -600,19 +642,19 @@
       </c>
       <c r="C4">
         <f ca="1">1-C3</f>
-        <v>0.51371723350831178</v>
+        <v>0.22680988972550931</v>
       </c>
       <c r="D4">
         <f ca="1">C4^2</f>
-        <v>0.26390539600343332</v>
-      </c>
-      <c r="E4" t="e">
+        <v>5.144272607729769E-2</v>
+      </c>
+      <c r="E4">
         <f t="array" aca="1" ref="E4:F4" ca="1">_xll.MONTE.STDEV(D4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F4" t="e">
+        <v>0.33408297440915841</v>
+      </c>
+      <c r="F4">
         <f ca="1"/>
-        <v>#NAME?</v>
+        <v>0.29901157934028644</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.45">
@@ -621,15 +663,15 @@
       </c>
       <c r="D5">
         <f ca="1">AVERAGE(D3:D4)</f>
-        <v>0.25018816249512155</v>
-      </c>
-      <c r="E5" t="e">
+        <v>0.32463283635178841</v>
+      </c>
+      <c r="E5">
         <f t="array" aca="1" ref="E5:F5" ca="1">_xll.MONTE.STDEV(D5)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" t="e">
+        <v>0.33382423850708492</v>
+      </c>
+      <c r="F5">
         <f ca="1"/>
-        <v>#NAME?</v>
+        <v>7.4585943101902613E-2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.45">
@@ -683,11 +725,12 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <f ca="1">NORMSINV(RAND())</f>
+        <v>-0.97834610413963774</v>
       </c>
       <c r="D14">
-        <f>-C14</f>
-        <v>0</v>
+        <f ca="1">-C14</f>
+        <v>0.97834610413963774</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>18</v>
@@ -697,23 +740,55 @@
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C15">
+        <f ca="1">f*EXP(sigma*SQRT(t)*C14 - (sigma^2)*t/2)</f>
+        <v>90.227618822715499</v>
+      </c>
+      <c r="D15">
+        <f ca="1">f*EXP(sigma*SQRT(t)*D14 - (sigma^2)*t/2)</f>
+        <v>109.72802415349958</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C16">
+        <f ca="1">MAX(k-C15,0)</f>
+        <v>9.7723811772845011</v>
+      </c>
+      <c r="D16">
+        <f ca="1">MAX(k-D15,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f ca="1">AVERAGE(C16:D16)</f>
+        <v>4.8861905886422505</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C17" cm="1">
+        <f t="array" aca="1" ref="C17" ca="1">_xll.MONTE.MEAN(C16)</f>
+        <v>4.0278657565045117</v>
+      </c>
+      <c r="D17" cm="1">
+        <f t="array" aca="1" ref="D17" ca="1">_xll.MONTE.MEAN(D16)</f>
+        <v>3.9317803702120377</v>
+      </c>
+      <c r="E17">
+        <f ca="1">AVERAGE(C17:D17)</f>
+        <v>3.9798230633582747</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
         <v>3</v>
       </c>
@@ -721,22 +796,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C22" t="e">
-        <f t="array" aca="1" ref="C22:D22" ca="1">monte.stdev(C16)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D22" t="e">
+      <c r="C22">
+        <f t="array" aca="1" ref="C22:D22" ca="1">_xll.MONTE.STDEV(C16)</f>
+        <v>4.0272393498948018</v>
+      </c>
+      <c r="D22">
         <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+        <v>5.5204090632600025</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B23" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C23">
+        <f t="array" aca="1" ref="C23:D23" ca="1">_xll.MONTE.STDEV(E16)</f>
+        <v>3.9795098600534322</v>
+      </c>
+      <c r="D23">
+        <f ca="1"/>
+        <v>2.654384145013986</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D24">
+        <f ca="1">D22/D23</f>
+        <v>2.0797325336762493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>